<commit_message>
export correlation matrix in EDA
</commit_message>
<xml_diff>
--- a/lu/processed_data/lasso_coef_imp.xlsx
+++ b/lu/processed_data/lasso_coef_imp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luyu/Dropbox/nycdsa/projects/proj3_houseprice/lu/processed_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B1B413BB-224F-E644-B4C6-C8035D2FD4C9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9394C5B-1DB7-D141-8E44-92A0FBC14B2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33000" yWindow="1060" windowWidth="28040" windowHeight="17440" xr2:uid="{4386FD0A-989C-EF4D-8032-12F7BD59F081}"/>
+    <workbookView xWindow="-15460" yWindow="1220" windowWidth="19040" windowHeight="17440" xr2:uid="{4386FD0A-989C-EF4D-8032-12F7BD59F081}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -522,11 +522,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22F039D2-D7BB-364F-8DD3-E4E34DA0039A}">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17.5" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>